<commit_message>
updated Gantt chart after discussion with mentors on 4/22/2020
</commit_message>
<xml_diff>
--- a/doc/Ganttchart_data.xlsx
+++ b/doc/Ganttchart_data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laura\Desktop\DIRECT\Capstone\ai_semiconductors\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B888847-FCBE-410C-B1AF-7C649925EE52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E03BA0-16B7-478D-81BA-3A3FCDE634A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18230" yWindow="2315" windowWidth="1920" windowHeight="1200" xr2:uid="{39CDD02A-CF22-45E9-9E33-1B53688FC745}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" activeTab="1" xr2:uid="{39CDD02A-CF22-45E9-9E33-1B53688FC745}"/>
   </bookViews>
   <sheets>
     <sheet name="200413" sheetId="1" r:id="rId1"/>
+    <sheet name="200422" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
   <si>
     <t>Task</t>
   </si>
@@ -44,16 +45,58 @@
     <t>End Date</t>
   </si>
   <si>
-    <t>Finding correlation between descriptors and outputs</t>
-  </si>
-  <si>
-    <t>Initial ML exploration (NN, RF, KRR)</t>
-  </si>
-  <si>
-    <t>Training model with data</t>
-  </si>
-  <si>
     <t>Have model completed</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Overall</t>
+  </si>
+  <si>
+    <t>Descriptor/Property correlation</t>
+  </si>
+  <si>
+    <t>ML exploration (NN, RF, KRR)</t>
+  </si>
+  <si>
+    <t>Initial data</t>
+  </si>
+  <si>
+    <t>Train models with data</t>
+  </si>
+  <si>
+    <t>Train models with DFT data</t>
+  </si>
+  <si>
+    <t>Total data</t>
+  </si>
+  <si>
+    <t>ML exploration (NN, RFR, KRR)</t>
+  </si>
+  <si>
+    <t>Test models with mixed alloy data</t>
+  </si>
+  <si>
+    <t>Brainstorm more descriptors</t>
+  </si>
+  <si>
+    <t>Lit Review</t>
+  </si>
+  <si>
+    <t>Bonus</t>
+  </si>
+  <si>
+    <t>Clean DFT data: outliers, normalize</t>
+  </si>
+  <si>
+    <t>Descriptor importance: remove unecessary</t>
+  </si>
+  <si>
+    <t>Train models with new DFT data (NN, RFR, LASSO, GPR)</t>
+  </si>
+  <si>
+    <t>Expected improvement:informed selection of new training data</t>
   </si>
 </sst>
 </file>
@@ -61,7 +104,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="mm/dd/yy;@"/>
+    <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -92,10 +135,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,20 +456,121 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57CBC46A-D69D-4404-A282-FB6A913D6CEF}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="A6:C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="43.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.2265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.2265625" customWidth="1"/>
-    <col min="5" max="6" width="17.86328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.81640625" customWidth="1"/>
+    <col min="2" max="2" width="9.31640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.2265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.2265625" customWidth="1"/>
+    <col min="6" max="7" width="17.86328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2">
+        <v>43934</v>
+      </c>
+      <c r="D2" s="2">
+        <v>43943</v>
+      </c>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2">
+        <v>43936</v>
+      </c>
+      <c r="D3" s="2">
+        <v>43950</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2">
+        <v>43936</v>
+      </c>
+      <c r="D4" s="2">
+        <v>43950</v>
+      </c>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="2">
+        <v>43987</v>
+      </c>
+      <c r="D5" s="2">
+        <v>44001</v>
+      </c>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{830960EC-7007-4F32-B7F8-0FBF670D1324}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="1" max="1" width="43.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.31640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.2265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.75">
@@ -431,66 +578,156 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="2">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2">
         <v>43934</v>
       </c>
-      <c r="C2" s="2">
+      <c r="D2" s="2">
         <v>43943</v>
       </c>
-      <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2">
         <v>43936</v>
       </c>
-      <c r="C3" s="2">
-        <v>43950</v>
-      </c>
-      <c r="D3" s="2"/>
+      <c r="D3" s="2">
+        <v>43943</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2">
+        <v>43936</v>
+      </c>
+      <c r="D4" s="2">
+        <v>43943</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="2">
+        <v>43943</v>
+      </c>
+      <c r="D5" s="2">
+        <v>43950</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="2">
+        <v>43945</v>
+      </c>
+      <c r="D6" s="2">
+        <v>43950</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="A7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="2">
+        <v>43945</v>
+      </c>
+      <c r="D7" s="1">
+        <v>43957</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="2">
+        <v>43964</v>
+      </c>
+      <c r="D8" s="1">
+        <v>43971</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="2">
+        <v>43966</v>
+      </c>
+      <c r="D9" s="1">
+        <v>43973</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="A10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="2">
+        <v>43971</v>
+      </c>
+      <c r="D10" s="1">
+        <v>43979</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2">
-        <v>43936</v>
-      </c>
-      <c r="C4" s="2">
-        <v>43950</v>
-      </c>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.75">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2">
+      <c r="C11" s="2">
         <v>43987</v>
       </c>
-      <c r="C5" s="2">
+      <c r="D11" s="2">
         <v>44001</v>
       </c>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.75">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Gantt chart update from 5/1/2020
</commit_message>
<xml_diff>
--- a/doc/Ganttchart_data.xlsx
+++ b/doc/Ganttchart_data.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laura\Desktop\DIRECT\Capstone\ai_semiconductors\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E03BA0-16B7-478D-81BA-3A3FCDE634A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E6812B9-0A84-4F3B-B594-99CFB66FDF75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" activeTab="1" xr2:uid="{39CDD02A-CF22-45E9-9E33-1B53688FC745}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" activeTab="2" xr2:uid="{39CDD02A-CF22-45E9-9E33-1B53688FC745}"/>
   </bookViews>
   <sheets>
     <sheet name="200413" sheetId="1" r:id="rId1"/>
     <sheet name="200422" sheetId="2" r:id="rId2"/>
+    <sheet name="200501" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="25">
   <si>
     <t>Task</t>
   </si>
@@ -97,6 +98,18 @@
   </si>
   <si>
     <t>Expected improvement:informed selection of new training data</t>
+  </si>
+  <si>
+    <t>Data Visualization: PCA, KNN, MDS</t>
+  </si>
+  <si>
+    <t>Expanded dataset (12k points) exploration</t>
+  </si>
+  <si>
+    <t>Expanded data</t>
+  </si>
+  <si>
+    <t>Expected improvement: informed selection of new training data</t>
   </si>
 </sst>
 </file>
@@ -561,8 +574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{830960EC-7007-4F32-B7F8-0FBF670D1324}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -730,4 +743,207 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2978932-4FF5-439D-90E5-B8D3B874C320}">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="1" max="1" width="57.90625" customWidth="1"/>
+    <col min="2" max="2" width="12.76953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.2265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2">
+        <v>43934</v>
+      </c>
+      <c r="D2" s="2">
+        <v>43943</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2">
+        <v>43936</v>
+      </c>
+      <c r="D3" s="2">
+        <v>43943</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2">
+        <v>43936</v>
+      </c>
+      <c r="D4" s="2">
+        <v>43943</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="2">
+        <v>43943</v>
+      </c>
+      <c r="D5" s="2">
+        <v>43950</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="2">
+        <v>43945</v>
+      </c>
+      <c r="D6" s="2">
+        <v>43950</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="2">
+        <v>43945</v>
+      </c>
+      <c r="D7" s="1">
+        <v>43957</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="2">
+        <v>43964</v>
+      </c>
+      <c r="D8" s="1">
+        <v>43971</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="2">
+        <v>43950</v>
+      </c>
+      <c r="D9" s="1">
+        <v>43957</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="2">
+        <v>43950</v>
+      </c>
+      <c r="D10" s="1">
+        <v>43964</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="2">
+        <v>43966</v>
+      </c>
+      <c r="D11" s="1">
+        <v>43973</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="2">
+        <v>43971</v>
+      </c>
+      <c r="D12" s="1">
+        <v>43979</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="2">
+        <v>43987</v>
+      </c>
+      <c r="D13" s="2">
+        <v>44001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
5/19/20 update to Gantt chart
</commit_message>
<xml_diff>
--- a/doc/Ganttchart_data.xlsx
+++ b/doc/Ganttchart_data.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laura\Desktop\DIRECT\Capstone\ai_semiconductors\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E6812B9-0A84-4F3B-B594-99CFB66FDF75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D050361-7B7B-41FF-A23E-257B0F7A6E88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" activeTab="2" xr2:uid="{39CDD02A-CF22-45E9-9E33-1B53688FC745}"/>
+    <workbookView xWindow="-28920" yWindow="-4290" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{39CDD02A-CF22-45E9-9E33-1B53688FC745}"/>
   </bookViews>
   <sheets>
     <sheet name="200413" sheetId="1" r:id="rId1"/>
     <sheet name="200422" sheetId="2" r:id="rId2"/>
     <sheet name="200501" sheetId="3" r:id="rId3"/>
+    <sheet name="200515" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="30">
   <si>
     <t>Task</t>
   </si>
@@ -106,10 +107,25 @@
     <t>Expanded dataset (12k points) exploration</t>
   </si>
   <si>
-    <t>Expanded data</t>
-  </si>
-  <si>
     <t>Expected improvement: informed selection of new training data</t>
+  </si>
+  <si>
+    <t>Chemical space</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outlier detection and removal </t>
+  </si>
+  <si>
+    <t>Outlier detection and removal: PCA, KNN</t>
+  </si>
+  <si>
+    <t>Model tuning with new descriptors</t>
+  </si>
+  <si>
+    <t>New Total data</t>
+  </si>
+  <si>
+    <t>Uncertainty prediction: all models</t>
   </si>
 </sst>
 </file>
@@ -749,14 +765,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2978932-4FF5-439D-90E5-B8D3B874C320}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="57.90625" customWidth="1"/>
-    <col min="2" max="2" width="12.76953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.90625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.2265625" bestFit="1" customWidth="1"/>
   </cols>
@@ -892,7 +908,7 @@
         <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C10" s="2">
         <v>43950</v>
@@ -917,7 +933,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A12" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>16</v>
@@ -940,6 +956,265 @@
         <v>43987</v>
       </c>
       <c r="D13" s="2">
+        <v>44001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{502BF6A5-AB71-4B0F-8CC4-AE47241D155F}">
+  <dimension ref="A1:D17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="1" max="1" width="56.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.2265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2">
+        <v>43934</v>
+      </c>
+      <c r="D2" s="2">
+        <v>43943</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2">
+        <v>43936</v>
+      </c>
+      <c r="D3" s="2">
+        <v>43943</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2">
+        <v>43936</v>
+      </c>
+      <c r="D4" s="2">
+        <v>43943</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="2">
+        <v>43943</v>
+      </c>
+      <c r="D5" s="2">
+        <v>43950</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="2">
+        <v>43945</v>
+      </c>
+      <c r="D6" s="2">
+        <v>43950</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="2">
+        <v>43945</v>
+      </c>
+      <c r="D7" s="1">
+        <v>43957</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="2">
+        <v>43973</v>
+      </c>
+      <c r="D8" s="1">
+        <v>43987</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="2">
+        <v>43950</v>
+      </c>
+      <c r="D9" s="1">
+        <v>43957</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="2">
+        <v>43950</v>
+      </c>
+      <c r="D10" s="1">
+        <v>43957</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="2">
+        <v>43950</v>
+      </c>
+      <c r="D11" s="1">
+        <v>43964</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="2">
+        <v>43957</v>
+      </c>
+      <c r="D12" s="1">
+        <v>43964</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="2">
+        <v>43957</v>
+      </c>
+      <c r="D13" s="1">
+        <v>43971</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="2">
+        <v>43966</v>
+      </c>
+      <c r="D14" s="1">
+        <v>43978</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="2">
+        <v>43966</v>
+      </c>
+      <c r="D15" s="1">
+        <v>43973</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A16" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="2">
+        <v>43971</v>
+      </c>
+      <c r="D16" s="1">
+        <v>43979</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="2">
+        <v>43987</v>
+      </c>
+      <c r="D17" s="2">
         <v>44001</v>
       </c>
     </row>

</xml_diff>